<commit_message>
Added RW, MTQ PD controller
</commit_message>
<xml_diff>
--- a/GantDiagram.xlsx
+++ b/GantDiagram.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlmartin/Dropbox/Masteroppgave/masterthesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E5D2FEE-3C97-6C43-BCD9-CFDB6379F09A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58231680-78FA-014F-A74D-676C69F5BC5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="22960" windowHeight="15000" xr2:uid="{2A600A6A-7C65-7B42-902C-238A440C13AF}"/>
   </bookViews>
@@ -154,7 +154,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,6 +165,12 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -241,7 +247,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -256,9 +262,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -266,6 +269,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -588,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B497B8-EA11-174C-9012-8910C7FAE568}">
   <dimension ref="A1:AG26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="117" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,70 +620,70 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6">
+      <c r="B1" s="9">
         <v>7</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9">
         <v>8</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6">
+      <c r="E1" s="9"/>
+      <c r="F1" s="9">
         <v>9</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6">
+      <c r="G1" s="9"/>
+      <c r="H1" s="9">
         <v>10</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6">
+      <c r="I1" s="9"/>
+      <c r="J1" s="9">
         <v>11</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6">
+      <c r="K1" s="9"/>
+      <c r="L1" s="9">
         <v>12</v>
       </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6">
+      <c r="M1" s="9"/>
+      <c r="N1" s="9">
         <v>13</v>
       </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6">
+      <c r="O1" s="9"/>
+      <c r="P1" s="9">
         <v>14</v>
       </c>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6">
+      <c r="Q1" s="9"/>
+      <c r="R1" s="10">
         <v>15</v>
       </c>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6">
+      <c r="S1" s="10"/>
+      <c r="T1" s="9">
         <v>16</v>
       </c>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6">
+      <c r="U1" s="9"/>
+      <c r="V1" s="9">
         <v>17</v>
       </c>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6">
+      <c r="W1" s="9"/>
+      <c r="X1" s="9">
         <v>18</v>
       </c>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6">
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9">
         <v>19</v>
       </c>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6">
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9">
         <v>20</v>
       </c>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6">
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9">
         <v>21</v>
       </c>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6">
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9">
         <v>22</v>
       </c>
-      <c r="AG1" s="6"/>
+      <c r="AG1" s="9"/>
     </row>
     <row r="2" spans="1:33" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -687,8 +705,8 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
@@ -708,7 +726,7 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -724,8 +742,8 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
@@ -742,18 +760,18 @@
       <c r="AG3" s="1"/>
     </row>
     <row r="4" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -761,8 +779,8 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
@@ -783,14 +801,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -798,8 +816,8 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
@@ -823,11 +841,11 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="1"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -835,8 +853,8 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
@@ -864,16 +882,16 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
@@ -909,8 +927,8 @@
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
       <c r="T8" s="5"/>
       <c r="U8" s="5"/>
       <c r="V8" s="5"/>
@@ -930,7 +948,7 @@
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="9"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -946,8 +964,8 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
@@ -967,7 +985,7 @@
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="7"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -983,8 +1001,8 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
@@ -1004,10 +1022,10 @@
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1020,8 +1038,8 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
@@ -1041,10 +1059,10 @@
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1057,8 +1075,8 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
@@ -1078,7 +1096,7 @@
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="7"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1094,8 +1112,8 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
@@ -1131,8 +1149,8 @@
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
       <c r="T14" s="5"/>
       <c r="U14" s="5"/>
       <c r="V14" s="5"/>
@@ -1154,12 +1172,8 @@
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1168,8 +1182,8 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
@@ -1194,19 +1208,18 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
@@ -1228,11 +1241,11 @@
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="1"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1242,8 +1255,8 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
@@ -1279,8 +1292,8 @@
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
       <c r="T18" s="5"/>
       <c r="U18" s="5"/>
       <c r="V18" s="5"/>
@@ -1310,14 +1323,14 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
@@ -1349,12 +1362,12 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
@@ -1390,8 +1403,8 @@
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
       <c r="T21" s="5"/>
       <c r="U21" s="5"/>
       <c r="V21" s="5"/>
@@ -1425,10 +1438,10 @@
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
@@ -1462,10 +1475,10 @@
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
@@ -1501,10 +1514,10 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
@@ -1538,10 +1551,10 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
@@ -1591,6 +1604,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="AD1:AE1"/>
     <mergeCell ref="AF1:AG1"/>
     <mergeCell ref="R1:S1"/>
@@ -1599,14 +1620,6 @@
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>